<commit_message>
Review VGM und Softwarekonzept
</commit_message>
<xml_diff>
--- a/ergebnisse/phase_1/Risikoanalyse.xlsx
+++ b/ergebnisse/phase_1/Risikoanalyse.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9302174-92B0-40DA-97A3-F14C7ADC64F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EFDB0E-85FB-467F-B9EF-B75003329BEE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,88 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{3F22ACE3-50A1-441F-BD01-8338D40D3FAE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Einbindung der GF fest einplanen</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{B9139D0C-C960-4A79-B1EE-92542C3120B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Einbeziehung/Informieren des Betriebsrates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{32F6125D-63F5-4B9B-B901-E27627B1312F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Aufstellen eines Kommunikationsplans</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
@@ -162,13 +244,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -217,7 +312,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -226,10 +321,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -251,14 +346,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CB78BA2E-95A2-40E0-9825-78DC4F07A432}" name="Tabelle1" displayName="Tabelle1" ref="A1:H51" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CB78BA2E-95A2-40E0-9825-78DC4F07A432}" name="Tabelle1" displayName="Tabelle1" ref="A1:H51" totalsRowShown="0" dataDxfId="8">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{EFE9D6C3-BA62-411D-B367-F4976B23181D}" name="Nr" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{CAEFEE30-9963-4A36-8E08-A7A925ADFD39}" name="Kategorie" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{93AC5BDB-D599-4567-B026-27A79C048DAE}" name="Risikobezeichnung" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{8073ED10-2B18-4A59-97DD-278FC9824AFF}" name="Mögliche Folgen / Tragweite" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{EFE9D6C3-BA62-411D-B367-F4976B23181D}" name="Nr" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{CAEFEE30-9963-4A36-8E08-A7A925ADFD39}" name="Kategorie" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{93AC5BDB-D599-4567-B026-27A79C048DAE}" name="Risikobezeichnung" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{8073ED10-2B18-4A59-97DD-278FC9824AFF}" name="Mögliche Folgen / Tragweite" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{F0B86906-4E29-4419-8E4A-4CE2B840B4D9}" name="Schadenshöhe" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{DBDD93D3-B9F1-4E72-8252-E4059CC26A99}" name="Eintrittswahrscheinlichkeit" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{DBDD93D3-B9F1-4E72-8252-E4059CC26A99}" name="Eintrittswahrscheinlichkeit" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{C0E41586-C2E7-435C-A6FA-19AB5C2AE027}" name="Eintrittsindikatoren" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{A3268568-F7FE-435A-A115-C9F57AE007BA}" name="Gegenmaßnahmen" dataDxfId="0"/>
   </tableColumns>
@@ -528,26 +623,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.21875" customWidth="1"/>
-    <col min="8" max="8" width="56.44140625" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="56.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,7 +668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -602,7 +697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -631,7 +726,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -656,7 +751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -681,7 +776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -703,7 +798,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -725,7 +820,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -747,7 +842,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -769,7 +864,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -787,7 +882,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -799,7 +894,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -811,7 +906,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -823,7 +918,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -835,7 +930,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -847,7 +942,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -859,7 +954,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -871,7 +966,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -883,7 +978,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -895,7 +990,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -907,7 +1002,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -919,7 +1014,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -931,7 +1026,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -943,7 +1038,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -955,7 +1050,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -967,7 +1062,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -979,7 +1074,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -991,7 +1086,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1003,7 +1098,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1015,7 +1110,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1027,7 +1122,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1039,7 +1134,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1051,7 +1146,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1063,7 +1158,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1075,7 +1170,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1087,7 +1182,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1099,7 +1194,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1111,7 +1206,7 @@
       <c r="G37" s="4"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1123,7 +1218,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1135,7 +1230,7 @@
       <c r="G39" s="4"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1147,7 +1242,7 @@
       <c r="G40" s="4"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1159,7 +1254,7 @@
       <c r="G41" s="4"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1171,7 +1266,7 @@
       <c r="G42" s="4"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1183,7 +1278,7 @@
       <c r="G43" s="4"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1195,7 +1290,7 @@
       <c r="G44" s="4"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1207,7 +1302,7 @@
       <c r="G45" s="4"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1219,7 +1314,7 @@
       <c r="G46" s="4"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1231,7 +1326,7 @@
       <c r="G47" s="4"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1243,7 +1338,7 @@
       <c r="G48" s="4"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1255,7 +1350,7 @@
       <c r="G49" s="4"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -1267,7 +1362,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="3"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1281,8 +1376,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1307,24 +1403,24 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>

</xml_diff>